<commit_message>
Versão enviada para análise Rodolfo.
</commit_message>
<xml_diff>
--- a/10-planejamento/cronograma/Detalhamento-Atividades-Dissertacao.xlsx
+++ b/10-planejamento/cronograma/Detalhamento-Atividades-Dissertacao.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>DETALHAMENTO  DAS ATIVIDADES DISSERTAÇÃO</t>
   </si>
@@ -35,6 +35,81 @@
   </si>
   <si>
     <t>Mapeamento Sistemático da Literatura</t>
+  </si>
+  <si>
+    <t>Identificar a necessidade da Revisão</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>Especificar questões de pesquisa</t>
+  </si>
+  <si>
+    <t>Desenvolver o Protocolo da Revisão</t>
+  </si>
+  <si>
+    <t>Selecionar  Estudos Primários</t>
+  </si>
+  <si>
+    <t>Extrair e sintetizar dados dos estudos primários</t>
+  </si>
+  <si>
+    <t>Redigir documento com os resultados da Revisão</t>
+  </si>
+  <si>
+    <t>Caracterização das Funcionalidades das Ferramentas</t>
+  </si>
+  <si>
+    <t>Selecionar as ferramentas utilizadas no estudo</t>
+  </si>
+  <si>
+    <t>Coletar o manual do usuários das ferramentas</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Sintetizar as funcionalidades das ferramentas</t>
+  </si>
+  <si>
+    <t>Pesquisa com Profissionais (Survey)</t>
+  </si>
+  <si>
+    <t>Definir critérios de escolha da população</t>
+  </si>
+  <si>
+    <t>Preparar questionário</t>
+  </si>
+  <si>
+    <t>Para Fazer</t>
+  </si>
+  <si>
+    <t>Realizar um piloto do survey</t>
+  </si>
+  <si>
+    <t>Realizar o survey com a população escolhida</t>
+  </si>
+  <si>
+    <t>Sintetizar e analisar o resultado do survey</t>
+  </si>
+  <si>
+    <t>Extensões para as Ferramentas</t>
+  </si>
+  <si>
+    <t>Definir o tipo extensão a ser desenvolvida</t>
+  </si>
+  <si>
+    <t>Desenvolver a extensão</t>
+  </si>
+  <si>
+    <t>Planejar experimento para avaliação da extensão</t>
+  </si>
+  <si>
+    <t>Coletar dados da avaliação da extensão</t>
+  </si>
+  <si>
+    <t>Analisar dados da avaliação da extensão</t>
   </si>
 </sst>
 </file>
@@ -45,7 +120,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="MM/YY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -66,13 +141,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -112,10 +180,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="double"/>
+      <right style="double"/>
+      <top style="double"/>
+      <bottom style="double"/>
       <diagonal/>
     </border>
   </borders>
@@ -144,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -153,20 +221,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -186,21 +266,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A8"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4132653061224"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -222,41 +301,192 @@
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.566666666666667" right="0.39375" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>